<commit_message>
Broken html links in profiles page
</commit_message>
<xml_diff>
--- a/docs/CareConnect-MedicationAdministration-1.xlsx
+++ b/docs/CareConnect-MedicationAdministration-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6692" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6692" uniqueCount="563">
   <si>
     <t>Path</t>
   </si>
@@ -591,9 +591,6 @@
   </si>
   <si>
     <t>There are many sets  of identifiers.  To perform matching of two identifiers, we need to know what set we're dealing with. The system identifies a particular set of unique identifiers.</t>
-  </si>
-  <si>
-    <t>http://www.acme.com/identifiers/patient or urn:ietf:rfc:3986 if the Identifier.value itself is a full uri</t>
   </si>
   <si>
     <t>Identifier.system</t>
@@ -4600,43 +4597,43 @@
         <v>36</v>
       </c>
       <c r="S27" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="T27" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="U27" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="V27" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="W27" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="X27" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Y27" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Z27" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AA27" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AB27" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AC27" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AD27" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AE27" t="s" s="2">
         <v>185</v>
-      </c>
-      <c r="T27" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="U27" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="V27" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="W27" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="X27" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="Y27" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="Z27" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AA27" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AB27" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AC27" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AD27" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AE27" t="s" s="2">
-        <v>186</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>37</v>
@@ -4653,7 +4650,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4679,13 +4676,13 @@
         <v>109</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="L28" t="s" s="2">
         <v>188</v>
       </c>
-      <c r="L28" t="s" s="2">
+      <c r="M28" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>190</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4699,43 +4696,43 @@
         <v>36</v>
       </c>
       <c r="S28" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="T28" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="U28" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="V28" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="W28" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="X28" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Y28" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Z28" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AA28" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AB28" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AC28" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AD28" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AE28" t="s" s="2">
         <v>191</v>
-      </c>
-      <c r="T28" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="U28" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="V28" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="W28" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="X28" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="Y28" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="Z28" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AA28" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AB28" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AC28" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AD28" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AE28" t="s" s="2">
-        <v>192</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>37</v>
@@ -4752,7 +4749,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4775,16 +4772,16 @@
         <v>46</v>
       </c>
       <c r="J29" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="K29" t="s" s="2">
         <v>194</v>
       </c>
-      <c r="K29" t="s" s="2">
+      <c r="L29" t="s" s="2">
         <v>195</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>196</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>197</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4834,7 +4831,7 @@
         <v>36</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>37</v>
@@ -4846,12 +4843,12 @@
         <v>52</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4950,7 +4947,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5049,7 +5046,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5072,16 +5069,16 @@
         <v>46</v>
       </c>
       <c r="J32" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="K32" t="s" s="2">
         <v>203</v>
       </c>
-      <c r="K32" t="s" s="2">
+      <c r="L32" t="s" s="2">
         <v>204</v>
       </c>
-      <c r="L32" t="s" s="2">
+      <c r="M32" t="s" s="2">
         <v>205</v>
-      </c>
-      <c r="M32" t="s" s="2">
-        <v>206</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -5131,16 +5128,16 @@
         <v>36</v>
       </c>
       <c r="AE32" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="AF32" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH32" t="s" s="2">
         <v>207</v>
-      </c>
-      <c r="AF32" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AG32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH32" t="s" s="2">
-        <v>208</v>
       </c>
       <c r="AI32" t="s" s="2">
         <v>53</v>
@@ -5148,7 +5145,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5171,69 +5168,69 @@
         <v>46</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K33" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="L33" t="s" s="2">
         <v>210</v>
       </c>
-      <c r="L33" t="s" s="2">
+      <c r="M33" t="s" s="2">
         <v>211</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>212</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>36</v>
       </c>
       <c r="P33" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="Q33" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="R33" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="S33" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="T33" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="U33" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="V33" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="W33" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="X33" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Y33" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Z33" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AA33" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AB33" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AC33" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AD33" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AE33" t="s" s="2">
         <v>213</v>
       </c>
-      <c r="Q33" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="R33" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="S33" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="T33" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="U33" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="V33" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="W33" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="X33" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="Y33" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="Z33" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AA33" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AB33" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AC33" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AD33" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AE33" t="s" s="2">
-        <v>214</v>
-      </c>
       <c r="AF33" t="s" s="2">
         <v>37</v>
       </c>
@@ -5241,7 +5238,7 @@
         <v>45</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>53</v>
@@ -5249,7 +5246,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5272,16 +5269,16 @@
         <v>46</v>
       </c>
       <c r="J34" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="K34" t="s" s="2">
         <v>216</v>
       </c>
-      <c r="K34" t="s" s="2">
+      <c r="L34" t="s" s="2">
         <v>217</v>
       </c>
-      <c r="L34" t="s" s="2">
+      <c r="M34" t="s" s="2">
         <v>218</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>219</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
@@ -5331,7 +5328,7 @@
         <v>36</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>37</v>
@@ -5343,12 +5340,12 @@
         <v>52</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5447,7 +5444,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5546,7 +5543,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5572,13 +5569,13 @@
         <v>109</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="M37" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
@@ -5628,16 +5625,16 @@
         <v>36</v>
       </c>
       <c r="AE37" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AF37" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH37" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AF37" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AG37" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH37" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>53</v>
@@ -5645,7 +5642,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5671,13 +5668,13 @@
         <v>105</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="L38" t="s" s="2">
+      <c r="M38" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
@@ -5727,7 +5724,7 @@
         <v>36</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>37</v>
@@ -5744,7 +5741,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5770,13 +5767,13 @@
         <v>109</v>
       </c>
       <c r="K39" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="L39" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="L39" t="s" s="2">
+      <c r="M39" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
@@ -5826,7 +5823,7 @@
         <v>36</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>37</v>
@@ -5843,7 +5840,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5866,16 +5863,16 @@
         <v>46</v>
       </c>
       <c r="J40" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="K40" t="s" s="2">
         <v>241</v>
       </c>
-      <c r="K40" t="s" s="2">
+      <c r="L40" t="s" s="2">
         <v>242</v>
       </c>
-      <c r="L40" t="s" s="2">
+      <c r="M40" t="s" s="2">
         <v>243</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>244</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
@@ -5925,7 +5922,7 @@
         <v>36</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>37</v>
@@ -5937,12 +5934,12 @@
         <v>52</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6041,7 +6038,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6140,7 +6137,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6166,13 +6163,13 @@
         <v>109</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -6222,16 +6219,16 @@
         <v>36</v>
       </c>
       <c r="AE43" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AF43" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG43" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH43" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AF43" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AG43" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH43" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="AI43" t="s" s="2">
         <v>53</v>
@@ -6239,7 +6236,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6265,13 +6262,13 @@
         <v>105</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="L44" t="s" s="2">
+      <c r="M44" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="M44" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
@@ -6321,7 +6318,7 @@
         <v>36</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>37</v>
@@ -6338,7 +6335,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6364,13 +6361,13 @@
         <v>109</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="L45" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="L45" t="s" s="2">
+      <c r="M45" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
@@ -6420,7 +6417,7 @@
         <v>36</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>37</v>
@@ -6437,7 +6434,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6460,16 +6457,16 @@
         <v>46</v>
       </c>
       <c r="J46" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="K46" t="s" s="2">
         <v>251</v>
       </c>
-      <c r="K46" t="s" s="2">
+      <c r="L46" t="s" s="2">
         <v>252</v>
       </c>
-      <c r="L46" t="s" s="2">
-        <v>253</v>
-      </c>
       <c r="M46" t="s" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
@@ -6519,7 +6516,7 @@
         <v>36</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>37</v>
@@ -6531,12 +6528,12 @@
         <v>52</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6635,7 +6632,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6734,7 +6731,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6760,13 +6757,13 @@
         <v>109</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="L49" t="s" s="2">
+      <c r="M49" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="M49" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
@@ -6816,16 +6813,16 @@
         <v>36</v>
       </c>
       <c r="AE49" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AF49" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG49" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH49" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AF49" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AG49" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH49" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>53</v>
@@ -6833,7 +6830,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6859,13 +6856,13 @@
         <v>105</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L50" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="L50" t="s" s="2">
+      <c r="M50" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
@@ -6915,7 +6912,7 @@
         <v>36</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>37</v>
@@ -6932,7 +6929,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -6958,13 +6955,13 @@
         <v>109</v>
       </c>
       <c r="K51" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="L51" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="L51" t="s" s="2">
+      <c r="M51" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
@@ -7014,7 +7011,7 @@
         <v>36</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>37</v>
@@ -7031,7 +7028,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7057,13 +7054,13 @@
         <v>66</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="L52" t="s" s="2">
         <v>260</v>
       </c>
-      <c r="L52" t="s" s="2">
+      <c r="M52" t="s" s="2">
         <v>261</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>262</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
@@ -7092,11 +7089,11 @@
         <v>122</v>
       </c>
       <c r="X52" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="Y52" t="s" s="2">
         <v>263</v>
       </c>
-      <c r="Y52" t="s" s="2">
-        <v>264</v>
-      </c>
       <c r="Z52" t="s" s="2">
         <v>36</v>
       </c>
@@ -7113,7 +7110,7 @@
         <v>36</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>45</v>
@@ -7130,7 +7127,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7156,13 +7153,13 @@
         <v>127</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="L53" t="s" s="2">
         <v>266</v>
       </c>
-      <c r="L53" t="s" s="2">
+      <c r="M53" t="s" s="2">
         <v>267</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>268</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" t="s" s="2">
@@ -7188,14 +7185,14 @@
         <v>36</v>
       </c>
       <c r="W53" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="X53" t="s" s="2">
         <v>269</v>
       </c>
-      <c r="X53" t="s" s="2">
+      <c r="Y53" t="s" s="2">
         <v>270</v>
       </c>
-      <c r="Y53" t="s" s="2">
-        <v>271</v>
-      </c>
       <c r="Z53" t="s" s="2">
         <v>36</v>
       </c>
@@ -7212,7 +7209,7 @@
         <v>36</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>37</v>
@@ -7229,7 +7226,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7328,7 +7325,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7427,7 +7424,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7528,7 +7525,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7627,7 +7624,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7726,7 +7723,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7827,7 +7824,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -7926,7 +7923,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8027,7 +8024,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8128,7 +8125,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8229,7 +8226,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8330,10 +8327,10 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="B65" t="s" s="2">
         <v>283</v>
-      </c>
-      <c r="B65" t="s" s="2">
-        <v>284</v>
       </c>
       <c r="C65" t="s" s="2">
         <v>36</v>
@@ -8355,16 +8352,16 @@
         <v>46</v>
       </c>
       <c r="J65" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="K65" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="K65" t="s" s="2">
+      <c r="L65" t="s" s="2">
         <v>286</v>
       </c>
-      <c r="L65" t="s" s="2">
+      <c r="M65" t="s" s="2">
         <v>287</v>
-      </c>
-      <c r="M65" t="s" s="2">
-        <v>288</v>
       </c>
       <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
@@ -8390,31 +8387,31 @@
         <v>36</v>
       </c>
       <c r="W65" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="X65" t="s" s="2">
         <v>289</v>
       </c>
-      <c r="X65" t="s" s="2">
+      <c r="Y65" t="s" s="2">
         <v>290</v>
       </c>
-      <c r="Y65" t="s" s="2">
+      <c r="Z65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AA65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AB65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AC65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AD65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AE65" t="s" s="2">
         <v>291</v>
-      </c>
-      <c r="Z65" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AA65" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AB65" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AC65" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AD65" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AE65" t="s" s="2">
-        <v>292</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>45</v>
@@ -8431,7 +8428,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8454,16 +8451,16 @@
         <v>46</v>
       </c>
       <c r="J66" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="K66" t="s" s="2">
         <v>294</v>
       </c>
-      <c r="K66" t="s" s="2">
+      <c r="L66" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="L66" t="s" s="2">
-        <v>296</v>
-      </c>
       <c r="M66" t="s" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
@@ -8513,7 +8510,7 @@
         <v>36</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>45</v>
@@ -8525,12 +8522,12 @@
         <v>52</v>
       </c>
       <c r="AI66" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8629,7 +8626,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -8728,7 +8725,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -8754,13 +8751,13 @@
         <v>109</v>
       </c>
       <c r="K69" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="L69" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="L69" t="s" s="2">
+      <c r="M69" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="M69" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="N69" s="2"/>
       <c r="O69" t="s" s="2">
@@ -8810,16 +8807,16 @@
         <v>36</v>
       </c>
       <c r="AE69" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AF69" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG69" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH69" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AF69" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AG69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH69" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="AI69" t="s" s="2">
         <v>53</v>
@@ -8827,7 +8824,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -8853,13 +8850,13 @@
         <v>105</v>
       </c>
       <c r="K70" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L70" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="L70" t="s" s="2">
+      <c r="M70" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="M70" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="N70" s="2"/>
       <c r="O70" t="s" s="2">
@@ -8909,7 +8906,7 @@
         <v>36</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>37</v>
@@ -8926,7 +8923,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -8952,13 +8949,13 @@
         <v>109</v>
       </c>
       <c r="K71" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="L71" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="L71" t="s" s="2">
+      <c r="M71" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M71" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="N71" s="2"/>
       <c r="O71" t="s" s="2">
@@ -9008,7 +9005,7 @@
         <v>36</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>37</v>
@@ -9025,7 +9022,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9048,16 +9045,16 @@
         <v>36</v>
       </c>
       <c r="J72" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="K72" t="s" s="2">
         <v>303</v>
       </c>
-      <c r="K72" t="s" s="2">
+      <c r="L72" t="s" s="2">
         <v>304</v>
       </c>
-      <c r="L72" t="s" s="2">
-        <v>305</v>
-      </c>
       <c r="M72" t="s" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
@@ -9107,7 +9104,7 @@
         <v>36</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>37</v>
@@ -9119,12 +9116,12 @@
         <v>52</v>
       </c>
       <c r="AI72" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9223,7 +9220,7 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -9322,7 +9319,7 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -9348,13 +9345,13 @@
         <v>109</v>
       </c>
       <c r="K75" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="L75" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="L75" t="s" s="2">
+      <c r="M75" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="M75" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="N75" s="2"/>
       <c r="O75" t="s" s="2">
@@ -9404,16 +9401,16 @@
         <v>36</v>
       </c>
       <c r="AE75" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AF75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG75" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH75" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AF75" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AG75" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH75" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="AI75" t="s" s="2">
         <v>53</v>
@@ -9421,7 +9418,7 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -9447,13 +9444,13 @@
         <v>105</v>
       </c>
       <c r="K76" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L76" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="L76" t="s" s="2">
+      <c r="M76" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="M76" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="N76" s="2"/>
       <c r="O76" t="s" s="2">
@@ -9503,7 +9500,7 @@
         <v>36</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>37</v>
@@ -9520,7 +9517,7 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -9546,13 +9543,13 @@
         <v>109</v>
       </c>
       <c r="K77" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="L77" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="L77" t="s" s="2">
+      <c r="M77" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M77" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" t="s" s="2">
@@ -9602,7 +9599,7 @@
         <v>36</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>37</v>
@@ -9619,7 +9616,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -9642,16 +9639,16 @@
         <v>36</v>
       </c>
       <c r="J78" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="K78" t="s" s="2">
         <v>312</v>
       </c>
-      <c r="K78" t="s" s="2">
+      <c r="L78" t="s" s="2">
         <v>313</v>
       </c>
-      <c r="L78" t="s" s="2">
-        <v>314</v>
-      </c>
       <c r="M78" t="s" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N78" s="2"/>
       <c r="O78" t="s" s="2">
@@ -9701,7 +9698,7 @@
         <v>36</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>37</v>
@@ -9713,12 +9710,12 @@
         <v>52</v>
       </c>
       <c r="AI78" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -9817,7 +9814,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -9916,7 +9913,7 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -9942,13 +9939,13 @@
         <v>109</v>
       </c>
       <c r="K81" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="L81" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="L81" t="s" s="2">
+      <c r="M81" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="M81" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="N81" s="2"/>
       <c r="O81" t="s" s="2">
@@ -9998,16 +9995,16 @@
         <v>36</v>
       </c>
       <c r="AE81" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AF81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG81" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH81" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AF81" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AG81" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH81" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="AI81" t="s" s="2">
         <v>53</v>
@@ -10015,7 +10012,7 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -10041,13 +10038,13 @@
         <v>105</v>
       </c>
       <c r="K82" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L82" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="L82" t="s" s="2">
+      <c r="M82" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="M82" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="N82" s="2"/>
       <c r="O82" t="s" s="2">
@@ -10097,7 +10094,7 @@
         <v>36</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>37</v>
@@ -10114,7 +10111,7 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -10140,13 +10137,13 @@
         <v>109</v>
       </c>
       <c r="K83" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="L83" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="L83" t="s" s="2">
+      <c r="M83" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M83" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="N83" s="2"/>
       <c r="O83" t="s" s="2">
@@ -10196,7 +10193,7 @@
         <v>36</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>37</v>
@@ -10213,7 +10210,7 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -10236,13 +10233,13 @@
         <v>46</v>
       </c>
       <c r="J84" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="K84" t="s" s="2">
         <v>321</v>
       </c>
-      <c r="K84" t="s" s="2">
+      <c r="L84" t="s" s="2">
         <v>322</v>
-      </c>
-      <c r="L84" t="s" s="2">
-        <v>323</v>
       </c>
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
@@ -10293,7 +10290,7 @@
         <v>36</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>45</v>
@@ -10310,7 +10307,7 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
@@ -10333,13 +10330,13 @@
         <v>46</v>
       </c>
       <c r="J85" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="K85" t="s" s="2">
         <v>325</v>
       </c>
-      <c r="K85" t="s" s="2">
+      <c r="L85" t="s" s="2">
         <v>326</v>
-      </c>
-      <c r="L85" t="s" s="2">
-        <v>327</v>
       </c>
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
@@ -10390,7 +10387,7 @@
         <v>36</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AF85" t="s" s="2">
         <v>37</v>
@@ -10407,7 +10404,7 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -10506,7 +10503,7 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
@@ -10605,11 +10602,11 @@
     </row>
     <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" t="s" s="2">
@@ -10634,7 +10631,7 @@
         <v>101</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M88" t="s" s="2">
         <v>94</v>
@@ -10687,7 +10684,7 @@
         <v>36</v>
       </c>
       <c r="AE88" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AF88" t="s" s="2">
         <v>37</v>
@@ -10704,7 +10701,7 @@
     </row>
     <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s" s="2">
@@ -10727,16 +10724,16 @@
         <v>46</v>
       </c>
       <c r="J89" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="K89" t="s" s="2">
         <v>335</v>
       </c>
-      <c r="K89" t="s" s="2">
+      <c r="L89" t="s" s="2">
         <v>336</v>
       </c>
-      <c r="L89" t="s" s="2">
-        <v>337</v>
-      </c>
       <c r="M89" t="s" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N89" s="2"/>
       <c r="O89" t="s" s="2">
@@ -10786,7 +10783,7 @@
         <v>36</v>
       </c>
       <c r="AE89" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AF89" t="s" s="2">
         <v>45</v>
@@ -10798,12 +10795,12 @@
         <v>52</v>
       </c>
       <c r="AI89" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" t="s" s="2">
@@ -10902,7 +10899,7 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" t="s" s="2">
@@ -11001,7 +10998,7 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" t="s" s="2">
@@ -11027,13 +11024,13 @@
         <v>109</v>
       </c>
       <c r="K92" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="L92" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="L92" t="s" s="2">
+      <c r="M92" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="M92" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="N92" s="2"/>
       <c r="O92" t="s" s="2">
@@ -11083,16 +11080,16 @@
         <v>36</v>
       </c>
       <c r="AE92" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AF92" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG92" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH92" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AF92" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AG92" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH92" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="AI92" t="s" s="2">
         <v>53</v>
@@ -11100,7 +11097,7 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" t="s" s="2">
@@ -11126,13 +11123,13 @@
         <v>105</v>
       </c>
       <c r="K93" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L93" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="L93" t="s" s="2">
+      <c r="M93" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="M93" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="N93" s="2"/>
       <c r="O93" t="s" s="2">
@@ -11182,7 +11179,7 @@
         <v>36</v>
       </c>
       <c r="AE93" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF93" t="s" s="2">
         <v>37</v>
@@ -11199,7 +11196,7 @@
     </row>
     <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" t="s" s="2">
@@ -11225,13 +11222,13 @@
         <v>109</v>
       </c>
       <c r="K94" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="L94" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="L94" t="s" s="2">
+      <c r="M94" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M94" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="N94" s="2"/>
       <c r="O94" t="s" s="2">
@@ -11281,7 +11278,7 @@
         <v>36</v>
       </c>
       <c r="AE94" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF94" t="s" s="2">
         <v>37</v>
@@ -11298,7 +11295,7 @@
     </row>
     <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" t="s" s="2">
@@ -11321,16 +11318,16 @@
         <v>36</v>
       </c>
       <c r="J95" t="s" s="2">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K95" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="L95" t="s" s="2">
         <v>344</v>
       </c>
-      <c r="L95" t="s" s="2">
-        <v>345</v>
-      </c>
       <c r="M95" t="s" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N95" s="2"/>
       <c r="O95" t="s" s="2">
@@ -11380,7 +11377,7 @@
         <v>36</v>
       </c>
       <c r="AE95" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="AF95" t="s" s="2">
         <v>37</v>
@@ -11392,12 +11389,12 @@
         <v>52</v>
       </c>
       <c r="AI95" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="96" hidden="true">
       <c r="A96" t="s" s="2">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" t="s" s="2">
@@ -11496,7 +11493,7 @@
     </row>
     <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" t="s" s="2">
@@ -11595,7 +11592,7 @@
     </row>
     <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" t="s" s="2">
@@ -11621,13 +11618,13 @@
         <v>109</v>
       </c>
       <c r="K98" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="L98" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="L98" t="s" s="2">
+      <c r="M98" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="M98" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="N98" s="2"/>
       <c r="O98" t="s" s="2">
@@ -11677,16 +11674,16 @@
         <v>36</v>
       </c>
       <c r="AE98" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AF98" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG98" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH98" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AF98" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AG98" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH98" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="AI98" t="s" s="2">
         <v>53</v>
@@ -11694,7 +11691,7 @@
     </row>
     <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" t="s" s="2">
@@ -11720,13 +11717,13 @@
         <v>105</v>
       </c>
       <c r="K99" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L99" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="L99" t="s" s="2">
+      <c r="M99" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="M99" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="N99" s="2"/>
       <c r="O99" t="s" s="2">
@@ -11776,7 +11773,7 @@
         <v>36</v>
       </c>
       <c r="AE99" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF99" t="s" s="2">
         <v>37</v>
@@ -11793,7 +11790,7 @@
     </row>
     <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" t="s" s="2">
@@ -11819,13 +11816,13 @@
         <v>109</v>
       </c>
       <c r="K100" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="L100" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="L100" t="s" s="2">
+      <c r="M100" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M100" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="N100" s="2"/>
       <c r="O100" t="s" s="2">
@@ -11875,7 +11872,7 @@
         <v>36</v>
       </c>
       <c r="AE100" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF100" t="s" s="2">
         <v>37</v>
@@ -11892,7 +11889,7 @@
     </row>
     <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" t="s" s="2">
@@ -11918,20 +11915,20 @@
         <v>168</v>
       </c>
       <c r="K101" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="L101" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="L101" t="s" s="2">
+      <c r="M101" t="s" s="2">
         <v>353</v>
-      </c>
-      <c r="M101" t="s" s="2">
-        <v>354</v>
       </c>
       <c r="N101" s="2"/>
       <c r="O101" t="s" s="2">
         <v>36</v>
       </c>
       <c r="P101" t="s" s="2">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="Q101" t="s" s="2">
         <v>36</v>
@@ -11976,7 +11973,7 @@
         <v>36</v>
       </c>
       <c r="AE101" t="s" s="2">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AF101" t="s" s="2">
         <v>37</v>
@@ -11993,7 +11990,7 @@
     </row>
     <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" t="s" s="2">
@@ -12019,13 +12016,13 @@
         <v>127</v>
       </c>
       <c r="K102" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="L102" t="s" s="2">
         <v>357</v>
       </c>
-      <c r="L102" t="s" s="2">
-        <v>358</v>
-      </c>
       <c r="M102" t="s" s="2">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="N102" s="2"/>
       <c r="O102" t="s" s="2">
@@ -12051,14 +12048,14 @@
         <v>36</v>
       </c>
       <c r="W102" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="X102" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="Y102" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="Y102" t="s" s="2">
-        <v>360</v>
-      </c>
       <c r="Z102" t="s" s="2">
         <v>36</v>
       </c>
@@ -12075,7 +12072,7 @@
         <v>36</v>
       </c>
       <c r="AE102" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AF102" t="s" s="2">
         <v>37</v>
@@ -12084,7 +12081,7 @@
         <v>38</v>
       </c>
       <c r="AH102" t="s" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="AI102" t="s" s="2">
         <v>53</v>
@@ -12092,7 +12089,7 @@
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" t="s" s="2">
@@ -12191,7 +12188,7 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" t="s" s="2">
@@ -12290,7 +12287,7 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" t="s" s="2">
@@ -12391,7 +12388,7 @@
     </row>
     <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B106" s="2"/>
       <c r="C106" t="s" s="2">
@@ -12490,7 +12487,7 @@
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B107" s="2"/>
       <c r="C107" t="s" s="2">
@@ -12589,7 +12586,7 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" t="s" s="2">
@@ -12690,7 +12687,7 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" t="s" s="2">
@@ -12789,7 +12786,7 @@
     </row>
     <row r="110" hidden="true">
       <c r="A110" t="s" s="2">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" t="s" s="2">
@@ -12890,7 +12887,7 @@
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B111" s="2"/>
       <c r="C111" t="s" s="2">
@@ -12991,7 +12988,7 @@
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" t="s" s="2">
@@ -13092,7 +13089,7 @@
     </row>
     <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" t="s" s="2">
@@ -13193,7 +13190,7 @@
     </row>
     <row r="114" hidden="true">
       <c r="A114" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" t="s" s="2">
@@ -13219,13 +13216,13 @@
         <v>127</v>
       </c>
       <c r="K114" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="L114" t="s" s="2">
         <v>374</v>
       </c>
-      <c r="L114" t="s" s="2">
-        <v>375</v>
-      </c>
       <c r="M114" t="s" s="2">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="N114" s="2"/>
       <c r="O114" t="s" s="2">
@@ -13251,14 +13248,14 @@
         <v>36</v>
       </c>
       <c r="W114" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="X114" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="Y114" t="s" s="2">
         <v>376</v>
       </c>
-      <c r="Y114" t="s" s="2">
-        <v>377</v>
-      </c>
       <c r="Z114" t="s" s="2">
         <v>36</v>
       </c>
@@ -13275,7 +13272,7 @@
         <v>36</v>
       </c>
       <c r="AE114" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AF114" t="s" s="2">
         <v>37</v>
@@ -13284,7 +13281,7 @@
         <v>38</v>
       </c>
       <c r="AH114" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AI114" t="s" s="2">
         <v>53</v>
@@ -13292,7 +13289,7 @@
     </row>
     <row r="115" hidden="true">
       <c r="A115" t="s" s="2">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B115" s="2"/>
       <c r="C115" t="s" s="2">
@@ -13391,7 +13388,7 @@
     </row>
     <row r="116" hidden="true">
       <c r="A116" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B116" s="2"/>
       <c r="C116" t="s" s="2">
@@ -13490,7 +13487,7 @@
     </row>
     <row r="117" hidden="true">
       <c r="A117" t="s" s="2">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" t="s" s="2">
@@ -13591,7 +13588,7 @@
     </row>
     <row r="118" hidden="true">
       <c r="A118" t="s" s="2">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" t="s" s="2">
@@ -13690,7 +13687,7 @@
     </row>
     <row r="119" hidden="true">
       <c r="A119" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" t="s" s="2">
@@ -13789,7 +13786,7 @@
     </row>
     <row r="120" hidden="true">
       <c r="A120" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" t="s" s="2">
@@ -13890,7 +13887,7 @@
     </row>
     <row r="121" hidden="true">
       <c r="A121" t="s" s="2">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B121" s="2"/>
       <c r="C121" t="s" s="2">
@@ -13989,7 +13986,7 @@
     </row>
     <row r="122" hidden="true">
       <c r="A122" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B122" s="2"/>
       <c r="C122" t="s" s="2">
@@ -14090,7 +14087,7 @@
     </row>
     <row r="123" hidden="true">
       <c r="A123" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" t="s" s="2">
@@ -14191,7 +14188,7 @@
     </row>
     <row r="124" hidden="true">
       <c r="A124" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B124" s="2"/>
       <c r="C124" t="s" s="2">
@@ -14292,7 +14289,7 @@
     </row>
     <row r="125" hidden="true">
       <c r="A125" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B125" s="2"/>
       <c r="C125" t="s" s="2">
@@ -14393,7 +14390,7 @@
     </row>
     <row r="126" hidden="true">
       <c r="A126" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B126" s="2"/>
       <c r="C126" t="s" s="2">
@@ -14416,16 +14413,16 @@
         <v>36</v>
       </c>
       <c r="J126" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="K126" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="K126" t="s" s="2">
+      <c r="L126" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="L126" t="s" s="2">
+      <c r="M126" t="s" s="2">
         <v>393</v>
-      </c>
-      <c r="M126" t="s" s="2">
-        <v>394</v>
       </c>
       <c r="N126" s="2"/>
       <c r="O126" t="s" s="2">
@@ -14475,7 +14472,7 @@
         <v>36</v>
       </c>
       <c r="AE126" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AF126" t="s" s="2">
         <v>37</v>
@@ -14487,12 +14484,12 @@
         <v>52</v>
       </c>
       <c r="AI126" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="127" hidden="true">
       <c r="A127" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" t="s" s="2">
@@ -14591,7 +14588,7 @@
     </row>
     <row r="128" hidden="true">
       <c r="A128" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" t="s" s="2">
@@ -14690,7 +14687,7 @@
     </row>
     <row r="129" hidden="true">
       <c r="A129" t="s" s="2">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B129" s="2"/>
       <c r="C129" t="s" s="2">
@@ -14716,13 +14713,13 @@
         <v>109</v>
       </c>
       <c r="K129" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="L129" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="L129" t="s" s="2">
+      <c r="M129" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="M129" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="N129" s="2"/>
       <c r="O129" t="s" s="2">
@@ -14772,16 +14769,16 @@
         <v>36</v>
       </c>
       <c r="AE129" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AF129" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG129" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH129" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AF129" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AG129" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH129" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="AI129" t="s" s="2">
         <v>53</v>
@@ -14789,7 +14786,7 @@
     </row>
     <row r="130" hidden="true">
       <c r="A130" t="s" s="2">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B130" s="2"/>
       <c r="C130" t="s" s="2">
@@ -14815,13 +14812,13 @@
         <v>105</v>
       </c>
       <c r="K130" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L130" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="L130" t="s" s="2">
+      <c r="M130" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="M130" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="N130" s="2"/>
       <c r="O130" t="s" s="2">
@@ -14871,7 +14868,7 @@
         <v>36</v>
       </c>
       <c r="AE130" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF130" t="s" s="2">
         <v>37</v>
@@ -14888,7 +14885,7 @@
     </row>
     <row r="131" hidden="true">
       <c r="A131" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B131" s="2"/>
       <c r="C131" t="s" s="2">
@@ -14914,13 +14911,13 @@
         <v>109</v>
       </c>
       <c r="K131" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="L131" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="L131" t="s" s="2">
+      <c r="M131" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M131" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="N131" s="2"/>
       <c r="O131" t="s" s="2">
@@ -14970,7 +14967,7 @@
         <v>36</v>
       </c>
       <c r="AE131" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF131" t="s" s="2">
         <v>37</v>
@@ -14987,7 +14984,7 @@
     </row>
     <row r="132" hidden="true">
       <c r="A132" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B132" s="2"/>
       <c r="C132" t="s" s="2">
@@ -15010,16 +15007,16 @@
         <v>36</v>
       </c>
       <c r="J132" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="K132" t="s" s="2">
         <v>401</v>
       </c>
-      <c r="K132" t="s" s="2">
+      <c r="L132" t="s" s="2">
         <v>402</v>
       </c>
-      <c r="L132" t="s" s="2">
-        <v>403</v>
-      </c>
       <c r="M132" t="s" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N132" s="2"/>
       <c r="O132" t="s" s="2">
@@ -15069,7 +15066,7 @@
         <v>36</v>
       </c>
       <c r="AE132" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AF132" t="s" s="2">
         <v>37</v>
@@ -15081,12 +15078,12 @@
         <v>52</v>
       </c>
       <c r="AI132" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="133" hidden="true">
       <c r="A133" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B133" s="2"/>
       <c r="C133" t="s" s="2">
@@ -15185,7 +15182,7 @@
     </row>
     <row r="134" hidden="true">
       <c r="A134" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" t="s" s="2">
@@ -15284,7 +15281,7 @@
     </row>
     <row r="135" hidden="true">
       <c r="A135" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" t="s" s="2">
@@ -15310,13 +15307,13 @@
         <v>109</v>
       </c>
       <c r="K135" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="L135" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="L135" t="s" s="2">
+      <c r="M135" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="M135" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="N135" s="2"/>
       <c r="O135" t="s" s="2">
@@ -15366,16 +15363,16 @@
         <v>36</v>
       </c>
       <c r="AE135" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AF135" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG135" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH135" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AF135" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AG135" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH135" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="AI135" t="s" s="2">
         <v>53</v>
@@ -15383,7 +15380,7 @@
     </row>
     <row r="136" hidden="true">
       <c r="A136" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B136" s="2"/>
       <c r="C136" t="s" s="2">
@@ -15409,13 +15406,13 @@
         <v>105</v>
       </c>
       <c r="K136" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L136" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="L136" t="s" s="2">
+      <c r="M136" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="M136" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="N136" s="2"/>
       <c r="O136" t="s" s="2">
@@ -15465,7 +15462,7 @@
         <v>36</v>
       </c>
       <c r="AE136" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF136" t="s" s="2">
         <v>37</v>
@@ -15482,7 +15479,7 @@
     </row>
     <row r="137" hidden="true">
       <c r="A137" t="s" s="2">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B137" s="2"/>
       <c r="C137" t="s" s="2">
@@ -15508,13 +15505,13 @@
         <v>109</v>
       </c>
       <c r="K137" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="L137" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="L137" t="s" s="2">
+      <c r="M137" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M137" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="N137" s="2"/>
       <c r="O137" t="s" s="2">
@@ -15564,7 +15561,7 @@
         <v>36</v>
       </c>
       <c r="AE137" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF137" t="s" s="2">
         <v>37</v>
@@ -15581,7 +15578,7 @@
     </row>
     <row r="138" hidden="true">
       <c r="A138" t="s" s="2">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B138" s="2"/>
       <c r="C138" t="s" s="2">
@@ -15604,16 +15601,16 @@
         <v>36</v>
       </c>
       <c r="J138" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="K138" t="s" s="2">
         <v>410</v>
       </c>
-      <c r="K138" t="s" s="2">
+      <c r="L138" t="s" s="2">
         <v>411</v>
       </c>
-      <c r="L138" t="s" s="2">
-        <v>412</v>
-      </c>
       <c r="M138" t="s" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N138" s="2"/>
       <c r="O138" t="s" s="2">
@@ -15663,7 +15660,7 @@
         <v>36</v>
       </c>
       <c r="AE138" t="s" s="2">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AF138" t="s" s="2">
         <v>37</v>
@@ -15675,12 +15672,12 @@
         <v>52</v>
       </c>
       <c r="AI138" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="139" hidden="true">
       <c r="A139" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B139" s="2"/>
       <c r="C139" t="s" s="2">
@@ -15779,7 +15776,7 @@
     </row>
     <row r="140" hidden="true">
       <c r="A140" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B140" s="2"/>
       <c r="C140" t="s" s="2">
@@ -15878,7 +15875,7 @@
     </row>
     <row r="141" hidden="true">
       <c r="A141" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B141" s="2"/>
       <c r="C141" t="s" s="2">
@@ -15904,13 +15901,13 @@
         <v>109</v>
       </c>
       <c r="K141" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="L141" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="L141" t="s" s="2">
+      <c r="M141" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="M141" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="N141" s="2"/>
       <c r="O141" t="s" s="2">
@@ -15960,16 +15957,16 @@
         <v>36</v>
       </c>
       <c r="AE141" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AF141" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG141" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH141" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AF141" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AG141" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH141" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="AI141" t="s" s="2">
         <v>53</v>
@@ -15977,7 +15974,7 @@
     </row>
     <row r="142" hidden="true">
       <c r="A142" t="s" s="2">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B142" s="2"/>
       <c r="C142" t="s" s="2">
@@ -16003,13 +16000,13 @@
         <v>105</v>
       </c>
       <c r="K142" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L142" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="L142" t="s" s="2">
+      <c r="M142" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="M142" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="N142" s="2"/>
       <c r="O142" t="s" s="2">
@@ -16059,7 +16056,7 @@
         <v>36</v>
       </c>
       <c r="AE142" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF142" t="s" s="2">
         <v>37</v>
@@ -16076,7 +16073,7 @@
     </row>
     <row r="143" hidden="true">
       <c r="A143" t="s" s="2">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" t="s" s="2">
@@ -16102,13 +16099,13 @@
         <v>109</v>
       </c>
       <c r="K143" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="L143" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="L143" t="s" s="2">
+      <c r="M143" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M143" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="N143" s="2"/>
       <c r="O143" t="s" s="2">
@@ -16158,7 +16155,7 @@
         <v>36</v>
       </c>
       <c r="AE143" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF143" t="s" s="2">
         <v>37</v>
@@ -16175,7 +16172,7 @@
     </row>
     <row r="144" hidden="true">
       <c r="A144" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" t="s" s="2">
@@ -16198,16 +16195,16 @@
         <v>36</v>
       </c>
       <c r="J144" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="K144" t="s" s="2">
         <v>419</v>
       </c>
-      <c r="K144" t="s" s="2">
+      <c r="L144" t="s" s="2">
         <v>420</v>
       </c>
-      <c r="L144" t="s" s="2">
+      <c r="M144" t="s" s="2">
         <v>421</v>
-      </c>
-      <c r="M144" t="s" s="2">
-        <v>422</v>
       </c>
       <c r="N144" s="2"/>
       <c r="O144" t="s" s="2">
@@ -16257,7 +16254,7 @@
         <v>36</v>
       </c>
       <c r="AE144" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AF144" t="s" s="2">
         <v>37</v>
@@ -16274,7 +16271,7 @@
     </row>
     <row r="145" hidden="true">
       <c r="A145" t="s" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" t="s" s="2">
@@ -16373,7 +16370,7 @@
     </row>
     <row r="146" hidden="true">
       <c r="A146" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B146" s="2"/>
       <c r="C146" t="s" s="2">
@@ -16472,7 +16469,7 @@
     </row>
     <row r="147" hidden="true">
       <c r="A147" t="s" s="2">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B147" s="2"/>
       <c r="C147" t="s" s="2">
@@ -16495,16 +16492,16 @@
         <v>46</v>
       </c>
       <c r="J147" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="K147" t="s" s="2">
         <v>426</v>
       </c>
-      <c r="K147" t="s" s="2">
+      <c r="L147" t="s" s="2">
         <v>427</v>
       </c>
-      <c r="L147" t="s" s="2">
-        <v>428</v>
-      </c>
       <c r="M147" t="s" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N147" s="2"/>
       <c r="O147" t="s" s="2">
@@ -16554,7 +16551,7 @@
         <v>36</v>
       </c>
       <c r="AE147" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AF147" t="s" s="2">
         <v>37</v>
@@ -16566,12 +16563,12 @@
         <v>52</v>
       </c>
       <c r="AI147" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="148" hidden="true">
       <c r="A148" t="s" s="2">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B148" s="2"/>
       <c r="C148" t="s" s="2">
@@ -16594,13 +16591,13 @@
         <v>46</v>
       </c>
       <c r="J148" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K148" t="s" s="2">
+        <v>430</v>
+      </c>
+      <c r="L148" t="s" s="2">
         <v>431</v>
-      </c>
-      <c r="L148" t="s" s="2">
-        <v>432</v>
       </c>
       <c r="M148" s="2"/>
       <c r="N148" s="2"/>
@@ -16651,7 +16648,7 @@
         <v>36</v>
       </c>
       <c r="AE148" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="AF148" t="s" s="2">
         <v>37</v>
@@ -16668,7 +16665,7 @@
     </row>
     <row r="149" hidden="true">
       <c r="A149" t="s" s="2">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B149" s="2"/>
       <c r="C149" t="s" s="2">
@@ -16694,10 +16691,10 @@
         <v>109</v>
       </c>
       <c r="K149" t="s" s="2">
+        <v>434</v>
+      </c>
+      <c r="L149" t="s" s="2">
         <v>435</v>
-      </c>
-      <c r="L149" t="s" s="2">
-        <v>436</v>
       </c>
       <c r="M149" t="s" s="2">
         <v>112</v>
@@ -16750,7 +16747,7 @@
         <v>36</v>
       </c>
       <c r="AE149" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AF149" t="s" s="2">
         <v>45</v>
@@ -16767,7 +16764,7 @@
     </row>
     <row r="150" hidden="true">
       <c r="A150" t="s" s="2">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B150" s="2"/>
       <c r="C150" t="s" s="2">
@@ -16790,13 +16787,13 @@
         <v>36</v>
       </c>
       <c r="J150" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K150" t="s" s="2">
+        <v>438</v>
+      </c>
+      <c r="L150" t="s" s="2">
         <v>439</v>
-      </c>
-      <c r="L150" t="s" s="2">
-        <v>440</v>
       </c>
       <c r="M150" s="2"/>
       <c r="N150" s="2"/>
@@ -16847,7 +16844,7 @@
         <v>36</v>
       </c>
       <c r="AE150" t="s" s="2">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AF150" t="s" s="2">
         <v>37</v>
@@ -16859,12 +16856,12 @@
         <v>52</v>
       </c>
       <c r="AI150" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="151" hidden="true">
       <c r="A151" t="s" s="2">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B151" s="2"/>
       <c r="C151" t="s" s="2">
@@ -16963,7 +16960,7 @@
     </row>
     <row r="152" hidden="true">
       <c r="A152" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B152" s="2"/>
       <c r="C152" t="s" s="2">
@@ -17062,11 +17059,11 @@
     </row>
     <row r="153" hidden="true">
       <c r="A153" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B153" s="2"/>
       <c r="C153" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D153" s="2"/>
       <c r="E153" t="s" s="2">
@@ -17091,7 +17088,7 @@
         <v>101</v>
       </c>
       <c r="L153" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M153" t="s" s="2">
         <v>94</v>
@@ -17144,7 +17141,7 @@
         <v>36</v>
       </c>
       <c r="AE153" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AF153" t="s" s="2">
         <v>37</v>
@@ -17161,7 +17158,7 @@
     </row>
     <row r="154" hidden="true">
       <c r="A154" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B154" s="2"/>
       <c r="C154" t="s" s="2">
@@ -17187,10 +17184,10 @@
         <v>109</v>
       </c>
       <c r="K154" t="s" s="2">
+        <v>445</v>
+      </c>
+      <c r="L154" t="s" s="2">
         <v>446</v>
-      </c>
-      <c r="L154" t="s" s="2">
-        <v>447</v>
       </c>
       <c r="M154" t="s" s="2">
         <v>112</v>
@@ -17243,7 +17240,7 @@
         <v>36</v>
       </c>
       <c r="AE154" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AF154" t="s" s="2">
         <v>37</v>
@@ -17260,7 +17257,7 @@
     </row>
     <row r="155" hidden="true">
       <c r="A155" t="s" s="2">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B155" s="2"/>
       <c r="C155" t="s" s="2">
@@ -17286,13 +17283,13 @@
         <v>127</v>
       </c>
       <c r="K155" t="s" s="2">
+        <v>448</v>
+      </c>
+      <c r="L155" t="s" s="2">
         <v>449</v>
       </c>
-      <c r="L155" t="s" s="2">
+      <c r="M155" t="s" s="2">
         <v>450</v>
-      </c>
-      <c r="M155" t="s" s="2">
-        <v>451</v>
       </c>
       <c r="N155" s="2"/>
       <c r="O155" t="s" s="2">
@@ -17318,14 +17315,14 @@
         <v>36</v>
       </c>
       <c r="W155" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="X155" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="Y155" t="s" s="2">
         <v>452</v>
       </c>
-      <c r="Y155" t="s" s="2">
-        <v>453</v>
-      </c>
       <c r="Z155" t="s" s="2">
         <v>36</v>
       </c>
@@ -17342,7 +17339,7 @@
         <v>36</v>
       </c>
       <c r="AE155" t="s" s="2">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="AF155" t="s" s="2">
         <v>37</v>
@@ -17359,7 +17356,7 @@
     </row>
     <row r="156" hidden="true">
       <c r="A156" t="s" s="2">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B156" s="2"/>
       <c r="C156" t="s" s="2">
@@ -17458,7 +17455,7 @@
     </row>
     <row r="157" hidden="true">
       <c r="A157" t="s" s="2">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B157" s="2"/>
       <c r="C157" t="s" s="2">
@@ -17557,7 +17554,7 @@
     </row>
     <row r="158" hidden="true">
       <c r="A158" t="s" s="2">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B158" s="2"/>
       <c r="C158" t="s" s="2">
@@ -17658,7 +17655,7 @@
     </row>
     <row r="159" hidden="true">
       <c r="A159" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B159" s="2"/>
       <c r="C159" t="s" s="2">
@@ -17757,7 +17754,7 @@
     </row>
     <row r="160" hidden="true">
       <c r="A160" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B160" s="2"/>
       <c r="C160" t="s" s="2">
@@ -17856,7 +17853,7 @@
     </row>
     <row r="161" hidden="true">
       <c r="A161" t="s" s="2">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B161" s="2"/>
       <c r="C161" t="s" s="2">
@@ -17957,7 +17954,7 @@
     </row>
     <row r="162" hidden="true">
       <c r="A162" t="s" s="2">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" t="s" s="2">
@@ -18056,7 +18053,7 @@
     </row>
     <row r="163" hidden="true">
       <c r="A163" t="s" s="2">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" t="s" s="2">
@@ -18157,7 +18154,7 @@
     </row>
     <row r="164" hidden="true">
       <c r="A164" t="s" s="2">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B164" s="2"/>
       <c r="C164" t="s" s="2">
@@ -18258,7 +18255,7 @@
     </row>
     <row r="165" hidden="true">
       <c r="A165" t="s" s="2">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" t="s" s="2">
@@ -18359,7 +18356,7 @@
     </row>
     <row r="166" hidden="true">
       <c r="A166" t="s" s="2">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B166" s="2"/>
       <c r="C166" t="s" s="2">
@@ -18460,7 +18457,7 @@
     </row>
     <row r="167" hidden="true">
       <c r="A167" t="s" s="2">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B167" s="2"/>
       <c r="C167" t="s" s="2">
@@ -18486,13 +18483,13 @@
         <v>127</v>
       </c>
       <c r="K167" t="s" s="2">
+        <v>465</v>
+      </c>
+      <c r="L167" t="s" s="2">
         <v>466</v>
       </c>
-      <c r="L167" t="s" s="2">
-        <v>467</v>
-      </c>
       <c r="M167" t="s" s="2">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="N167" s="2"/>
       <c r="O167" t="s" s="2">
@@ -18518,14 +18515,14 @@
         <v>36</v>
       </c>
       <c r="W167" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="X167" t="s" s="2">
+        <v>467</v>
+      </c>
+      <c r="Y167" t="s" s="2">
         <v>468</v>
       </c>
-      <c r="Y167" t="s" s="2">
-        <v>469</v>
-      </c>
       <c r="Z167" t="s" s="2">
         <v>36</v>
       </c>
@@ -18542,7 +18539,7 @@
         <v>36</v>
       </c>
       <c r="AE167" t="s" s="2">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AF167" t="s" s="2">
         <v>37</v>
@@ -18559,7 +18556,7 @@
     </row>
     <row r="168" hidden="true">
       <c r="A168" t="s" s="2">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B168" s="2"/>
       <c r="C168" t="s" s="2">
@@ -18658,7 +18655,7 @@
     </row>
     <row r="169" hidden="true">
       <c r="A169" t="s" s="2">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" t="s" s="2">
@@ -18757,7 +18754,7 @@
     </row>
     <row r="170" hidden="true">
       <c r="A170" t="s" s="2">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B170" s="2"/>
       <c r="C170" t="s" s="2">
@@ -18829,7 +18826,7 @@
         <v>36</v>
       </c>
       <c r="AA170" t="s" s="2">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="AB170" s="2"/>
       <c r="AC170" t="s" s="2">
@@ -18856,7 +18853,7 @@
     </row>
     <row r="171" hidden="true">
       <c r="A171" t="s" s="2">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B171" s="2"/>
       <c r="C171" t="s" s="2">
@@ -18955,7 +18952,7 @@
     </row>
     <row r="172" hidden="true">
       <c r="A172" t="s" s="2">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B172" s="2"/>
       <c r="C172" t="s" s="2">
@@ -19054,7 +19051,7 @@
     </row>
     <row r="173" hidden="true">
       <c r="A173" t="s" s="2">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B173" s="2"/>
       <c r="C173" t="s" s="2">
@@ -19155,7 +19152,7 @@
     </row>
     <row r="174" hidden="true">
       <c r="A174" t="s" s="2">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B174" s="2"/>
       <c r="C174" t="s" s="2">
@@ -19254,7 +19251,7 @@
     </row>
     <row r="175" hidden="true">
       <c r="A175" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B175" s="2"/>
       <c r="C175" t="s" s="2">
@@ -19355,7 +19352,7 @@
     </row>
     <row r="176" hidden="true">
       <c r="A176" t="s" s="2">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B176" s="2"/>
       <c r="C176" t="s" s="2">
@@ -19456,7 +19453,7 @@
     </row>
     <row r="177" hidden="true">
       <c r="A177" t="s" s="2">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B177" s="2"/>
       <c r="C177" t="s" s="2">
@@ -19557,10 +19554,10 @@
     </row>
     <row r="178" hidden="true">
       <c r="A178" t="s" s="2">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B178" t="s" s="2">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C178" t="s" s="2">
         <v>36</v>
@@ -19619,13 +19616,13 @@
         <v>36</v>
       </c>
       <c r="W178" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="X178" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="Y178" t="s" s="2">
         <v>482</v>
-      </c>
-      <c r="Y178" t="s" s="2">
-        <v>483</v>
       </c>
       <c r="Z178" t="s" s="2">
         <v>36</v>
@@ -19660,7 +19657,7 @@
     </row>
     <row r="179" hidden="true">
       <c r="A179" t="s" s="2">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B179" s="2"/>
       <c r="C179" t="s" s="2">
@@ -19759,7 +19756,7 @@
     </row>
     <row r="180" hidden="true">
       <c r="A180" t="s" s="2">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B180" s="2"/>
       <c r="C180" t="s" s="2">
@@ -19858,10 +19855,10 @@
     </row>
     <row r="181" hidden="true">
       <c r="A181" t="s" s="2">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B181" t="s" s="2">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C181" t="s" s="2">
         <v>90</v>
@@ -19883,13 +19880,13 @@
         <v>36</v>
       </c>
       <c r="J181" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="K181" t="s" s="2">
         <v>485</v>
       </c>
-      <c r="K181" t="s" s="2">
+      <c r="L181" t="s" s="2">
         <v>486</v>
-      </c>
-      <c r="L181" t="s" s="2">
-        <v>487</v>
       </c>
       <c r="M181" t="s" s="2">
         <v>94</v>
@@ -19959,7 +19956,7 @@
     </row>
     <row r="182" hidden="true">
       <c r="A182" t="s" s="2">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B182" s="2"/>
       <c r="C182" t="s" s="2">
@@ -20001,7 +19998,7 @@
       </c>
       <c r="P182" s="2"/>
       <c r="Q182" t="s" s="2">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="R182" t="s" s="2">
         <v>36</v>
@@ -20060,7 +20057,7 @@
     </row>
     <row r="183" hidden="true">
       <c r="A183" t="s" s="2">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B183" s="2"/>
       <c r="C183" t="s" s="2">
@@ -20159,7 +20156,7 @@
     </row>
     <row r="184" hidden="true">
       <c r="A184" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B184" s="2"/>
       <c r="C184" t="s" s="2">
@@ -20260,7 +20257,7 @@
     </row>
     <row r="185" hidden="true">
       <c r="A185" t="s" s="2">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B185" s="2"/>
       <c r="C185" t="s" s="2">
@@ -20361,7 +20358,7 @@
     </row>
     <row r="186" hidden="true">
       <c r="A186" t="s" s="2">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B186" s="2"/>
       <c r="C186" t="s" s="2">
@@ -20462,7 +20459,7 @@
     </row>
     <row r="187" hidden="true">
       <c r="A187" t="s" s="2">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B187" s="2"/>
       <c r="C187" t="s" s="2">
@@ -20563,7 +20560,7 @@
     </row>
     <row r="188" hidden="true">
       <c r="A188" t="s" s="2">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B188" s="2"/>
       <c r="C188" t="s" s="2">
@@ -20589,13 +20586,13 @@
         <v>127</v>
       </c>
       <c r="K188" t="s" s="2">
+        <v>490</v>
+      </c>
+      <c r="L188" t="s" s="2">
         <v>491</v>
       </c>
-      <c r="L188" t="s" s="2">
+      <c r="M188" t="s" s="2">
         <v>492</v>
-      </c>
-      <c r="M188" t="s" s="2">
-        <v>493</v>
       </c>
       <c r="N188" s="2"/>
       <c r="O188" t="s" s="2">
@@ -20621,14 +20618,14 @@
         <v>36</v>
       </c>
       <c r="W188" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="X188" t="s" s="2">
+        <v>493</v>
+      </c>
+      <c r="Y188" t="s" s="2">
         <v>494</v>
       </c>
-      <c r="Y188" t="s" s="2">
-        <v>495</v>
-      </c>
       <c r="Z188" t="s" s="2">
         <v>36</v>
       </c>
@@ -20645,7 +20642,7 @@
         <v>36</v>
       </c>
       <c r="AE188" t="s" s="2">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="AF188" t="s" s="2">
         <v>37</v>
@@ -20662,7 +20659,7 @@
     </row>
     <row r="189" hidden="true">
       <c r="A189" t="s" s="2">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B189" s="2"/>
       <c r="C189" t="s" s="2">
@@ -20761,7 +20758,7 @@
     </row>
     <row r="190" hidden="true">
       <c r="A190" t="s" s="2">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B190" s="2"/>
       <c r="C190" t="s" s="2">
@@ -20860,7 +20857,7 @@
     </row>
     <row r="191" hidden="true">
       <c r="A191" t="s" s="2">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B191" s="2"/>
       <c r="C191" t="s" s="2">
@@ -20961,7 +20958,7 @@
     </row>
     <row r="192" hidden="true">
       <c r="A192" t="s" s="2">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B192" s="2"/>
       <c r="C192" t="s" s="2">
@@ -21060,7 +21057,7 @@
     </row>
     <row r="193" hidden="true">
       <c r="A193" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B193" s="2"/>
       <c r="C193" t="s" s="2">
@@ -21159,7 +21156,7 @@
     </row>
     <row r="194" hidden="true">
       <c r="A194" t="s" s="2">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B194" s="2"/>
       <c r="C194" t="s" s="2">
@@ -21260,7 +21257,7 @@
     </row>
     <row r="195" hidden="true">
       <c r="A195" t="s" s="2">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B195" s="2"/>
       <c r="C195" t="s" s="2">
@@ -21359,7 +21356,7 @@
     </row>
     <row r="196" hidden="true">
       <c r="A196" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B196" s="2"/>
       <c r="C196" t="s" s="2">
@@ -21460,7 +21457,7 @@
     </row>
     <row r="197" hidden="true">
       <c r="A197" t="s" s="2">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B197" s="2"/>
       <c r="C197" t="s" s="2">
@@ -21561,7 +21558,7 @@
     </row>
     <row r="198" hidden="true">
       <c r="A198" t="s" s="2">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B198" s="2"/>
       <c r="C198" t="s" s="2">
@@ -21662,7 +21659,7 @@
     </row>
     <row r="199" hidden="true">
       <c r="A199" t="s" s="2">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B199" s="2"/>
       <c r="C199" t="s" s="2">
@@ -21763,7 +21760,7 @@
     </row>
     <row r="200" hidden="true">
       <c r="A200" t="s" s="2">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B200" s="2"/>
       <c r="C200" t="s" s="2">
@@ -21786,16 +21783,16 @@
         <v>36</v>
       </c>
       <c r="J200" t="s" s="2">
+        <v>507</v>
+      </c>
+      <c r="K200" t="s" s="2">
         <v>508</v>
       </c>
-      <c r="K200" t="s" s="2">
+      <c r="L200" t="s" s="2">
         <v>509</v>
       </c>
-      <c r="L200" t="s" s="2">
+      <c r="M200" t="s" s="2">
         <v>510</v>
-      </c>
-      <c r="M200" t="s" s="2">
-        <v>511</v>
       </c>
       <c r="N200" s="2"/>
       <c r="O200" t="s" s="2">
@@ -21845,7 +21842,7 @@
         <v>36</v>
       </c>
       <c r="AE200" t="s" s="2">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="AF200" t="s" s="2">
         <v>37</v>
@@ -21857,12 +21854,12 @@
         <v>52</v>
       </c>
       <c r="AI200" t="s" s="2">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="201" hidden="true">
       <c r="A201" t="s" s="2">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B201" s="2"/>
       <c r="C201" t="s" s="2">
@@ -21961,7 +21958,7 @@
     </row>
     <row r="202" hidden="true">
       <c r="A202" t="s" s="2">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B202" s="2"/>
       <c r="C202" t="s" s="2">
@@ -22060,7 +22057,7 @@
     </row>
     <row r="203" hidden="true">
       <c r="A203" t="s" s="2">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B203" s="2"/>
       <c r="C203" t="s" s="2">
@@ -22083,19 +22080,19 @@
         <v>46</v>
       </c>
       <c r="J203" t="s" s="2">
+        <v>515</v>
+      </c>
+      <c r="K203" t="s" s="2">
         <v>516</v>
       </c>
-      <c r="K203" t="s" s="2">
+      <c r="L203" t="s" s="2">
         <v>517</v>
       </c>
-      <c r="L203" t="s" s="2">
+      <c r="M203" t="s" s="2">
         <v>518</v>
       </c>
-      <c r="M203" t="s" s="2">
+      <c r="N203" t="s" s="2">
         <v>519</v>
-      </c>
-      <c r="N203" t="s" s="2">
-        <v>520</v>
       </c>
       <c r="O203" t="s" s="2">
         <v>36</v>
@@ -22144,7 +22141,7 @@
         <v>36</v>
       </c>
       <c r="AE203" t="s" s="2">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="AF203" t="s" s="2">
         <v>37</v>
@@ -22161,7 +22158,7 @@
     </row>
     <row r="204" hidden="true">
       <c r="A204" t="s" s="2">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B204" s="2"/>
       <c r="C204" t="s" s="2">
@@ -22187,22 +22184,22 @@
         <v>66</v>
       </c>
       <c r="K204" t="s" s="2">
+        <v>522</v>
+      </c>
+      <c r="L204" t="s" s="2">
         <v>523</v>
       </c>
-      <c r="L204" t="s" s="2">
+      <c r="M204" t="s" s="2">
         <v>524</v>
       </c>
-      <c r="M204" t="s" s="2">
+      <c r="N204" t="s" s="2">
         <v>525</v>
       </c>
-      <c r="N204" t="s" s="2">
+      <c r="O204" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="P204" t="s" s="2">
         <v>526</v>
-      </c>
-      <c r="O204" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="P204" t="s" s="2">
-        <v>527</v>
       </c>
       <c r="Q204" t="s" s="2">
         <v>36</v>
@@ -22226,28 +22223,28 @@
         <v>122</v>
       </c>
       <c r="X204" t="s" s="2">
+        <v>527</v>
+      </c>
+      <c r="Y204" t="s" s="2">
         <v>528</v>
       </c>
-      <c r="Y204" t="s" s="2">
+      <c r="Z204" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AA204" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AB204" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AC204" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AD204" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AE204" t="s" s="2">
         <v>529</v>
-      </c>
-      <c r="Z204" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AA204" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AB204" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AC204" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AD204" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AE204" t="s" s="2">
-        <v>530</v>
       </c>
       <c r="AF204" t="s" s="2">
         <v>37</v>
@@ -22264,7 +22261,7 @@
     </row>
     <row r="205" hidden="true">
       <c r="A205" t="s" s="2">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B205" s="2"/>
       <c r="C205" t="s" s="2">
@@ -22290,16 +22287,16 @@
         <v>109</v>
       </c>
       <c r="K205" t="s" s="2">
+        <v>531</v>
+      </c>
+      <c r="L205" t="s" s="2">
         <v>532</v>
-      </c>
-      <c r="L205" t="s" s="2">
-        <v>533</v>
       </c>
       <c r="M205" t="s" s="2">
         <v>112</v>
       </c>
       <c r="N205" t="s" s="2">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="O205" t="s" s="2">
         <v>36</v>
@@ -22348,7 +22345,7 @@
         <v>36</v>
       </c>
       <c r="AE205" t="s" s="2">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="AF205" t="s" s="2">
         <v>37</v>
@@ -22365,7 +22362,7 @@
     </row>
     <row r="206" hidden="true">
       <c r="A206" t="s" s="2">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B206" s="2"/>
       <c r="C206" t="s" s="2">
@@ -22391,16 +22388,16 @@
         <v>60</v>
       </c>
       <c r="K206" t="s" s="2">
+        <v>536</v>
+      </c>
+      <c r="L206" t="s" s="2">
         <v>537</v>
-      </c>
-      <c r="L206" t="s" s="2">
-        <v>538</v>
       </c>
       <c r="M206" t="s" s="2">
         <v>183</v>
       </c>
       <c r="N206" t="s" s="2">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="O206" t="s" s="2">
         <v>36</v>
@@ -22449,16 +22446,16 @@
         <v>36</v>
       </c>
       <c r="AE206" t="s" s="2">
+        <v>539</v>
+      </c>
+      <c r="AF206" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG206" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH206" t="s" s="2">
         <v>540</v>
-      </c>
-      <c r="AF206" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AG206" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH206" t="s" s="2">
-        <v>541</v>
       </c>
       <c r="AI206" t="s" s="2">
         <v>53</v>
@@ -22466,7 +22463,7 @@
     </row>
     <row r="207" hidden="true">
       <c r="A207" t="s" s="2">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B207" s="2"/>
       <c r="C207" t="s" s="2">
@@ -22492,16 +22489,16 @@
         <v>66</v>
       </c>
       <c r="K207" t="s" s="2">
+        <v>542</v>
+      </c>
+      <c r="L207" t="s" s="2">
         <v>543</v>
       </c>
-      <c r="L207" t="s" s="2">
+      <c r="M207" t="s" s="2">
         <v>544</v>
       </c>
-      <c r="M207" t="s" s="2">
+      <c r="N207" t="s" s="2">
         <v>545</v>
-      </c>
-      <c r="N207" t="s" s="2">
-        <v>546</v>
       </c>
       <c r="O207" t="s" s="2">
         <v>36</v>
@@ -22550,7 +22547,7 @@
         <v>36</v>
       </c>
       <c r="AE207" t="s" s="2">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AF207" t="s" s="2">
         <v>37</v>
@@ -22567,7 +22564,7 @@
     </row>
     <row r="208" hidden="true">
       <c r="A208" t="s" s="2">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B208" s="2"/>
       <c r="C208" t="s" s="2">
@@ -22590,16 +22587,16 @@
         <v>36</v>
       </c>
       <c r="J208" t="s" s="2">
+        <v>548</v>
+      </c>
+      <c r="K208" t="s" s="2">
         <v>549</v>
       </c>
-      <c r="K208" t="s" s="2">
+      <c r="L208" t="s" s="2">
         <v>550</v>
       </c>
-      <c r="L208" t="s" s="2">
+      <c r="M208" t="s" s="2">
         <v>551</v>
-      </c>
-      <c r="M208" t="s" s="2">
-        <v>552</v>
       </c>
       <c r="N208" s="2"/>
       <c r="O208" t="s" s="2">
@@ -22649,7 +22646,7 @@
         <v>36</v>
       </c>
       <c r="AE208" t="s" s="2">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AF208" t="s" s="2">
         <v>37</v>
@@ -22661,12 +22658,12 @@
         <v>52</v>
       </c>
       <c r="AI208" t="s" s="2">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="209" hidden="true">
       <c r="A209" t="s" s="2">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B209" s="2"/>
       <c r="C209" t="s" s="2">
@@ -22689,16 +22686,16 @@
         <v>36</v>
       </c>
       <c r="J209" t="s" s="2">
+        <v>554</v>
+      </c>
+      <c r="K209" t="s" s="2">
         <v>555</v>
       </c>
-      <c r="K209" t="s" s="2">
+      <c r="L209" t="s" s="2">
         <v>556</v>
       </c>
-      <c r="L209" t="s" s="2">
+      <c r="M209" t="s" s="2">
         <v>557</v>
-      </c>
-      <c r="M209" t="s" s="2">
-        <v>558</v>
       </c>
       <c r="N209" s="2"/>
       <c r="O209" t="s" s="2">
@@ -22748,7 +22745,7 @@
         <v>36</v>
       </c>
       <c r="AE209" t="s" s="2">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="AF209" t="s" s="2">
         <v>37</v>
@@ -22760,12 +22757,12 @@
         <v>52</v>
       </c>
       <c r="AI209" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="210" hidden="true">
       <c r="A210" t="s" s="2">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B210" s="2"/>
       <c r="C210" t="s" s="2">
@@ -22864,7 +22861,7 @@
     </row>
     <row r="211" hidden="true">
       <c r="A211" t="s" s="2">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B211" s="2"/>
       <c r="C211" t="s" s="2">
@@ -22963,7 +22960,7 @@
     </row>
     <row r="212" hidden="true">
       <c r="A212" t="s" s="2">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B212" s="2"/>
       <c r="C212" t="s" s="2">
@@ -22989,13 +22986,13 @@
         <v>109</v>
       </c>
       <c r="K212" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="L212" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="L212" t="s" s="2">
+      <c r="M212" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="M212" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="N212" s="2"/>
       <c r="O212" t="s" s="2">
@@ -23045,16 +23042,16 @@
         <v>36</v>
       </c>
       <c r="AE212" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AF212" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG212" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH212" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AF212" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AG212" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH212" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="AI212" t="s" s="2">
         <v>53</v>
@@ -23062,7 +23059,7 @@
     </row>
     <row r="213" hidden="true">
       <c r="A213" t="s" s="2">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B213" s="2"/>
       <c r="C213" t="s" s="2">
@@ -23088,13 +23085,13 @@
         <v>105</v>
       </c>
       <c r="K213" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L213" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="L213" t="s" s="2">
+      <c r="M213" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="M213" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="N213" s="2"/>
       <c r="O213" t="s" s="2">
@@ -23144,7 +23141,7 @@
         <v>36</v>
       </c>
       <c r="AE213" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF213" t="s" s="2">
         <v>37</v>
@@ -23161,7 +23158,7 @@
     </row>
     <row r="214" hidden="true">
       <c r="A214" t="s" s="2">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B214" s="2"/>
       <c r="C214" t="s" s="2">
@@ -23187,13 +23184,13 @@
         <v>109</v>
       </c>
       <c r="K214" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="L214" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="L214" t="s" s="2">
+      <c r="M214" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M214" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="N214" s="2"/>
       <c r="O214" t="s" s="2">
@@ -23243,7 +23240,7 @@
         <v>36</v>
       </c>
       <c r="AE214" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF214" t="s" s="2">
         <v>37</v>

</xml_diff>